<commit_message>
Optimize whole receive system to better work effectiveness
</commit_message>
<xml_diff>
--- a/twoDproject/digitalZoom/doc/数码变焦测试用例V2.0.xlsx
+++ b/twoDproject/digitalZoom/doc/数码变焦测试用例V2.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PycharmProjects\pythonProject_seevision\twoDproject\digitalZoom\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78EDEC79-62CB-46C4-9B1E-14D968AA1300}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B360E2E-55C2-40E6-A1FA-C163F48B859D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-960" yWindow="1095" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1870" uniqueCount="430">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1870" uniqueCount="431">
   <si>
     <t>测试项</t>
   </si>
@@ -1502,6 +1502,11 @@
   </si>
   <si>
     <t>Comment</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>放大时画面无卡顿，预览画面无明显延时、锯齿白屏黑屏等异常；
+预览画面放大1.3倍</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3415,7 +3420,7 @@
   <dimension ref="A1:H254"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3562,7 +3567,7 @@
         <v>38</v>
       </c>
       <c r="F7" s="55" t="s">
-        <v>73</v>
+        <v>430</v>
       </c>
       <c r="G7" s="55"/>
       <c r="H7" s="55"/>

</xml_diff>